<commit_message>
GaspreisMEMAP-File angepasst, Parameter Anlagen auf Server geändert
</commit_message>
<xml_diff>
--- a/CoSES/FC_data_series/Test1_Last_Preise.xlsx
+++ b/CoSES/FC_data_series/Test1_Last_Preise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Licklederer\meinOrdner\Interface_OPCUA_Server_Git\CoSES\FC_data_series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Arbeitsordner_MEMAP\02_Interface_OPCUA_Server\FC_data_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1375DC-F890-4086-81B2-56689021219E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F9ACE4-CDD7-411C-8862-C97F1D63DFD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8340" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="2955" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wärme" sheetId="2" r:id="rId1"/>
@@ -3228,8 +3228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22ABF507-AFCA-496B-A961-3E8F7099BD5D}">
   <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3268,7 +3268,7 @@
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="F4">
-        <v>9999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4246,8 +4246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAF7B51-A847-4EC9-8F79-6CFAC9CF8371}">
   <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F36"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4278,7 +4278,11 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="F4">
-        <v>0</v>
+        <v>9999</v>
+      </c>
+      <c r="G4">
+        <f>F4/100</f>
+        <v>99.99</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
@@ -4304,6 +4308,10 @@
         <f>ROUND(E5,1)</f>
         <v>7.1</v>
       </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G36" si="0">F5/100</f>
+        <v>7.0999999999999994E-2</v>
+      </c>
       <c r="L5" t="s">
         <v>7</v>
       </c>
@@ -4325,12 +4333,16 @@
         <v>214</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E36" si="0">$N$6*SIN($N$7*D6+$N$8)+$N$5</f>
+        <f t="shared" ref="E6:E36" si="1">$N$6*SIN($N$7*D6+$N$8)+$N$5</f>
         <v>7.1617709380946293</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F36" si="1">ROUND(E6,1)</f>
+        <f t="shared" ref="F6:F36" si="2">ROUND(E6,1)</f>
         <v>7.2</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>7.2000000000000008E-2</v>
       </c>
       <c r="L6" t="s">
         <v>9</v>
@@ -4354,12 +4366,16 @@
         <v>215</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.1983090468941242</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>7.2000000000000008E-2</v>
       </c>
       <c r="L7" t="s">
         <v>11</v>
@@ -4382,12 +4398,16 @@
         <v>216</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.1870743554768204</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.2</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>7.2000000000000008E-2</v>
       </c>
       <c r="L8" t="s">
         <v>10</v>
@@ -4410,12 +4430,16 @@
         <v>217</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.1285147555364041</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="L9" t="s">
         <v>12</v>
@@ -4439,12 +4463,16 @@
         <v>218</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.024964833527001</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -4461,12 +4489,16 @@
         <v>219</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.8805527980684431</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.9</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -4483,12 +4515,16 @@
         <v>220</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.7010359012959428</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.7</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -4505,12 +4541,16 @@
         <v>221</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.4935709153854804</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>6.5000000000000002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -4527,12 +4567,16 @@
         <v>222</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.2664288146316904</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.3</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>6.3E-2</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -4549,12 +4593,16 @@
         <v>223</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.0286650378032869</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -4571,15 +4619,19 @@
         <v>224</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.7897584763754146</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.8</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>5.7999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -4593,15 +4645,19 @@
         <v>225</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.5592335810389706</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.6</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>5.5999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>4</v>
       </c>
@@ -4615,15 +4671,19 @@
         <v>226</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.3462806519076267</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>4</v>
       </c>
@@ -4637,15 +4697,19 @@
         <v>227</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.1593894502540305</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>5.2000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>4</v>
       </c>
@@ -4659,15 +4723,19 @@
         <v>228</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.0060107385188255</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>4</v>
       </c>
@@ -4681,15 +4749,19 @@
         <v>265</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.9598885108870885</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>4</v>
       </c>
@@ -4703,15 +4775,19 @@
         <v>266</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.0995194170454736</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>4</v>
       </c>
@@ -4725,15 +4801,19 @@
         <v>267</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.2750496424154543</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.3</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>4</v>
       </c>
@@ -4747,15 +4827,19 @@
         <v>268</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.4794813508291789</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>4</v>
       </c>
@@ -4769,15 +4853,19 @@
         <v>269</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.7046644951937688</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.7</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>4</v>
       </c>
@@ -4791,15 +4879,19 @@
         <v>270</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.9416217341498951</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>5.9000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>4</v>
       </c>
@@ -4813,15 +4905,19 @@
         <v>271</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.1809063303422027</v>
       </c>
       <c r="F27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.2</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>6.2E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>4</v>
       </c>
@@ -4835,15 +4931,19 @@
         <v>272</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.4129787620267047</v>
       </c>
       <c r="F28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.4</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>4</v>
       </c>
@@ -4857,15 +4957,19 @@
         <v>273</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6285870336990387</v>
       </c>
       <c r="F29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.6</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>4</v>
       </c>
@@ -4879,15 +4983,19 @@
         <v>274</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.8191355239588916</v>
       </c>
       <c r="F30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.8</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>4</v>
       </c>
@@ -4901,15 +5009,19 @@
         <v>275</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.9770276658101213</v>
       </c>
       <c r="F31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>4</v>
       </c>
@@ -4923,15 +5035,19 @@
         <v>276</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.0959687978145976</v>
       </c>
       <c r="F32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>7.0999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>4</v>
       </c>
@@ -4945,15 +5061,19 @@
         <v>277</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.1712171123797424</v>
       </c>
       <c r="F33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.2</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>7.2000000000000008E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>4</v>
       </c>
@@ -4967,15 +5087,19 @@
         <v>278</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.1997726966636311</v>
       </c>
       <c r="F34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.2</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>7.2000000000000008E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>4</v>
       </c>
@@ -4989,15 +5113,19 @@
         <v>279</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.1804971296332232</v>
       </c>
       <c r="F35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.2</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>7.2000000000000008E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>4</v>
       </c>
@@ -5011,15 +5139,19 @@
         <v>280</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.114158867318455</v>
       </c>
       <c r="F36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>7.0999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>14</v>
       </c>

</xml_diff>